<commit_message>
update low/high -> lower/higher
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janghopark/Documents/GitHub/MDRO_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE92CCE2-F753-9F45-8FF7-59B03AC5826E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8612211-A44C-0D44-8C84-3D0C1EF8B720}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="998" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="-3000" windowWidth="38400" windowHeight="24000" tabRatio="998" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly CMIP5 tasmax (C) " sheetId="9" r:id="rId1"/>
@@ -389,150 +389,6 @@
     <t>Available upon request for academic research purpose only.</t>
   </si>
   <si>
-    <t>csiro-mk3-6-0.1.rcp26.high GPCD</t>
-  </si>
-  <si>
-    <t>csiro-mk3-6-0.1.rcp45.high GPCD</t>
-  </si>
-  <si>
-    <t>csiro-mk3-6-0.1.rcp60.high GPCD</t>
-  </si>
-  <si>
-    <t>csiro-mk3-6-0.1.rcp85.high GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-cm3.1.rcp26.high GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-cm3.1.rcp45.high GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-cm3.1.rcp60.high GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-cm3.1.rcp85.high GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-esm2m.1.rcp26.high GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-esm2m.1.rcp45.high GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-esm2m.1.rcp60.high GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-esm2m.1.rcp85.high GPCD</t>
-  </si>
-  <si>
-    <t>giss-e2-r.rcp26.high GPCD</t>
-  </si>
-  <si>
-    <t>giss-e2-r.rcp45.high GPCD</t>
-  </si>
-  <si>
-    <t>giss-e2-r.rcp60.high GPCD</t>
-  </si>
-  <si>
-    <t>giss-e2-r.rcp85.high GPCD</t>
-  </si>
-  <si>
-    <t>miroc-esm-chem.1.rcp26.high GPCD</t>
-  </si>
-  <si>
-    <t>miroc-esm-chem.1.rcp45.high GPCD</t>
-  </si>
-  <si>
-    <t>miroc-esm-chem.1.rcp60.high GPCD</t>
-  </si>
-  <si>
-    <t>miroc-esm-chem.1.rcp85.high GPCD</t>
-  </si>
-  <si>
-    <t>miroc5.1.rcp26.high GPCD</t>
-  </si>
-  <si>
-    <t>miroc5.1.rcp45.high GPCD</t>
-  </si>
-  <si>
-    <t>miroc5.1.rcp60.high GPCD</t>
-  </si>
-  <si>
-    <t>miroc5.1.rcp85.high GPCD</t>
-  </si>
-  <si>
-    <t>csiro-mk3-6-0.1.rcp26.low GPCD</t>
-  </si>
-  <si>
-    <t>csiro-mk3-6-0.1.rcp45.low GPCD</t>
-  </si>
-  <si>
-    <t>csiro-mk3-6-0.1.rcp60.low GPCD</t>
-  </si>
-  <si>
-    <t>csiro-mk3-6-0.1.rcp85.low GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-cm3.1.rcp26.low GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-cm3.1.rcp45.low GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-cm3.1.rcp60.low GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-cm3.1.rcp85.low GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-esm2m.1.rcp26.low GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-esm2m.1.rcp45.low GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-esm2m.1.rcp60.low GPCD</t>
-  </si>
-  <si>
-    <t>gfdl-esm2m.1.rcp85.low GPCD</t>
-  </si>
-  <si>
-    <t>giss-e2-r.rcp26.low GPCD</t>
-  </si>
-  <si>
-    <t>giss-e2-r.rcp45.low GPCD</t>
-  </si>
-  <si>
-    <t>giss-e2-r.rcp60.low GPCD</t>
-  </si>
-  <si>
-    <t>giss-e2-r.rcp85.low GPCD</t>
-  </si>
-  <si>
-    <t>miroc-esm-chem.1.rcp26.low GPCD</t>
-  </si>
-  <si>
-    <t>miroc-esm-chem.1.rcp45.low GPCD</t>
-  </si>
-  <si>
-    <t>miroc-esm-chem.1.rcp60.low GPCD</t>
-  </si>
-  <si>
-    <t>miroc-esm-chem.1.rcp85.low GPCD</t>
-  </si>
-  <si>
-    <t>miroc5.1.rcp26.low GPCD</t>
-  </si>
-  <si>
-    <t>miroc5.1.rcp45.low GPCD</t>
-  </si>
-  <si>
-    <t>miroc5.1.rcp60.low GPCD</t>
-  </si>
-  <si>
-    <t>miroc5.1.rcp85.low GPCD</t>
-  </si>
-  <si>
     <t>Climate model</t>
   </si>
   <si>
@@ -598,6 +454,150 @@
   <si>
     <t xml:space="preserve">Probability of Conditions </t>
   </si>
+  <si>
+    <t>csiro-mk3-6-0.1.rcp26.higher-GPCD</t>
+  </si>
+  <si>
+    <t>csiro-mk3-6-0.1.rcp45.higher-GPCD</t>
+  </si>
+  <si>
+    <t>csiro-mk3-6-0.1.rcp60.higher-GPCD</t>
+  </si>
+  <si>
+    <t>csiro-mk3-6-0.1.rcp85.higher-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-cm3.1.rcp26.higher-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-cm3.1.rcp45.higher-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-cm3.1.rcp60.higher-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-cm3.1.rcp85.higher-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-esm2m.1.rcp26.higher-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-esm2m.1.rcp45.higher-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-esm2m.1.rcp60.higher-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-esm2m.1.rcp85.higher-GPCD</t>
+  </si>
+  <si>
+    <t>giss-e2-r.rcp26.higher-GPCD</t>
+  </si>
+  <si>
+    <t>giss-e2-r.rcp45.higher-GPCD</t>
+  </si>
+  <si>
+    <t>giss-e2-r.rcp60.higher-GPCD</t>
+  </si>
+  <si>
+    <t>giss-e2-r.rcp85.higher-GPCD</t>
+  </si>
+  <si>
+    <t>miroc-esm-chem.1.rcp26.higher-GPCD</t>
+  </si>
+  <si>
+    <t>miroc-esm-chem.1.rcp45.higher-GPCD</t>
+  </si>
+  <si>
+    <t>miroc-esm-chem.1.rcp60.higher-GPCD</t>
+  </si>
+  <si>
+    <t>miroc-esm-chem.1.rcp85.higher-GPCD</t>
+  </si>
+  <si>
+    <t>miroc5.1.rcp26.higher-GPCD</t>
+  </si>
+  <si>
+    <t>miroc5.1.rcp45.higher-GPCD</t>
+  </si>
+  <si>
+    <t>miroc5.1.rcp60.higher-GPCD</t>
+  </si>
+  <si>
+    <t>miroc5.1.rcp85.higher-GPCD</t>
+  </si>
+  <si>
+    <t>csiro-mk3-6-0.1.rcp26.lower-GPCD</t>
+  </si>
+  <si>
+    <t>csiro-mk3-6-0.1.rcp45.lower-GPCD</t>
+  </si>
+  <si>
+    <t>csiro-mk3-6-0.1.rcp60.lower-GPCD</t>
+  </si>
+  <si>
+    <t>csiro-mk3-6-0.1.rcp85.lower-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-cm3.1.rcp26.lower-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-cm3.1.rcp45.lower-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-cm3.1.rcp60.lower-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-cm3.1.rcp85.lower-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-esm2m.1.rcp26.lower-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-esm2m.1.rcp45.lower-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-esm2m.1.rcp60.lower-GPCD</t>
+  </si>
+  <si>
+    <t>gfdl-esm2m.1.rcp85.lower-GPCD</t>
+  </si>
+  <si>
+    <t>giss-e2-r.rcp26.lower-GPCD</t>
+  </si>
+  <si>
+    <t>giss-e2-r.rcp45.lower-GPCD</t>
+  </si>
+  <si>
+    <t>giss-e2-r.rcp60.lower-GPCD</t>
+  </si>
+  <si>
+    <t>giss-e2-r.rcp85.lower-GPCD</t>
+  </si>
+  <si>
+    <t>miroc-esm-chem.1.rcp26.lower-GPCD</t>
+  </si>
+  <si>
+    <t>miroc-esm-chem.1.rcp45.lower-GPCD</t>
+  </si>
+  <si>
+    <t>miroc-esm-chem.1.rcp60.lower-GPCD</t>
+  </si>
+  <si>
+    <t>miroc-esm-chem.1.rcp85.lower-GPCD</t>
+  </si>
+  <si>
+    <t>miroc5.1.rcp26.lower-GPCD</t>
+  </si>
+  <si>
+    <t>miroc5.1.rcp45.lower-GPCD</t>
+  </si>
+  <si>
+    <t>miroc5.1.rcp60.lower-GPCD</t>
+  </si>
+  <si>
+    <t>miroc5.1.rcp85.lower-GPCD</t>
+  </si>
 </sst>
 </file>
 
@@ -605,7 +605,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -916,6 +916,21 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -925,33 +940,18 @@
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -64931,8 +64931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AW34"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AW1" sqref="AW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -64958,148 +64958,148 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="Z1" s="18" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="AA1" s="18" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="AB1" s="18" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="AC1" s="18" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="AD1" s="18" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="AE1" s="18" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="AF1" s="18" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="AG1" s="18" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="AH1" s="18" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="AI1" s="18" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="AJ1" s="18" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="AK1" s="18" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="AL1" s="18" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="AM1" s="18" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="AN1" s="18" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="AO1" s="18" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="AP1" s="18" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="AQ1" s="18" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="AR1" s="18" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="AS1" s="18" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="AT1" s="18" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="AU1" s="18" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="AV1" s="18" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="AW1" s="18" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.2">
@@ -70029,7 +70029,7 @@
   <dimension ref="A1:AQ28"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -70204,478 +70204,478 @@
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="37" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="26"/>
-      <c r="AH2" s="26"/>
-      <c r="AI2" s="26"/>
-      <c r="AJ2" s="26"/>
-      <c r="AK2" s="26"/>
-      <c r="AL2" s="26"/>
-      <c r="AM2" s="26"/>
-      <c r="AN2" s="26"/>
-      <c r="AO2" s="26"/>
-      <c r="AP2" s="26"/>
-      <c r="AQ2" s="26"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39"/>
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="39"/>
+      <c r="AN2" s="39"/>
+      <c r="AO2" s="39"/>
+      <c r="AP2" s="39"/>
+      <c r="AQ2" s="39"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="26"/>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="26"/>
-      <c r="AG3" s="26"/>
-      <c r="AH3" s="26"/>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="26"/>
-      <c r="AK3" s="26"/>
-      <c r="AL3" s="26"/>
-      <c r="AM3" s="26"/>
-      <c r="AN3" s="26"/>
-      <c r="AO3" s="26"/>
-      <c r="AP3" s="26"/>
-      <c r="AQ3" s="26"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="39"/>
+      <c r="AN3" s="39"/>
+      <c r="AO3" s="39"/>
+      <c r="AP3" s="39"/>
+      <c r="AQ3" s="39"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="26"/>
-      <c r="AJ4" s="26"/>
-      <c r="AK4" s="26"/>
-      <c r="AL4" s="26"/>
-      <c r="AM4" s="26"/>
-      <c r="AN4" s="26"/>
-      <c r="AO4" s="26"/>
-      <c r="AP4" s="26"/>
-      <c r="AQ4" s="26"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="39"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="39"/>
+      <c r="AA4" s="39"/>
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="39"/>
+      <c r="AD4" s="39"/>
+      <c r="AE4" s="39"/>
+      <c r="AF4" s="39"/>
+      <c r="AG4" s="39"/>
+      <c r="AH4" s="39"/>
+      <c r="AI4" s="39"/>
+      <c r="AJ4" s="39"/>
+      <c r="AK4" s="39"/>
+      <c r="AL4" s="39"/>
+      <c r="AM4" s="39"/>
+      <c r="AN4" s="39"/>
+      <c r="AO4" s="39"/>
+      <c r="AP4" s="39"/>
+      <c r="AQ4" s="39"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
-      <c r="AG5" s="26"/>
-      <c r="AH5" s="26"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-      <c r="AL5" s="26"/>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="26"/>
-      <c r="AP5" s="26"/>
-      <c r="AQ5" s="26"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39"/>
+      <c r="Z5" s="39"/>
+      <c r="AA5" s="39"/>
+      <c r="AB5" s="39"/>
+      <c r="AC5" s="39"/>
+      <c r="AD5" s="39"/>
+      <c r="AE5" s="39"/>
+      <c r="AF5" s="39"/>
+      <c r="AG5" s="39"/>
+      <c r="AH5" s="39"/>
+      <c r="AI5" s="39"/>
+      <c r="AJ5" s="39"/>
+      <c r="AK5" s="39"/>
+      <c r="AL5" s="39"/>
+      <c r="AM5" s="39"/>
+      <c r="AN5" s="39"/>
+      <c r="AO5" s="39"/>
+      <c r="AP5" s="39"/>
+      <c r="AQ5" s="39"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
-      <c r="AG6" s="26"/>
-      <c r="AH6" s="26"/>
-      <c r="AI6" s="26"/>
-      <c r="AJ6" s="26"/>
-      <c r="AK6" s="26"/>
-      <c r="AL6" s="26"/>
-      <c r="AM6" s="26"/>
-      <c r="AN6" s="26"/>
-      <c r="AO6" s="26"/>
-      <c r="AP6" s="26"/>
-      <c r="AQ6" s="26"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="39"/>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="39"/>
+      <c r="AH6" s="39"/>
+      <c r="AI6" s="39"/>
+      <c r="AJ6" s="39"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="39"/>
+      <c r="AM6" s="39"/>
+      <c r="AN6" s="39"/>
+      <c r="AO6" s="39"/>
+      <c r="AP6" s="39"/>
+      <c r="AQ6" s="39"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="26"/>
-      <c r="AE7" s="26"/>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="26"/>
-      <c r="AH7" s="26"/>
-      <c r="AI7" s="26"/>
-      <c r="AJ7" s="26"/>
-      <c r="AK7" s="26"/>
-      <c r="AL7" s="26"/>
-      <c r="AM7" s="26"/>
-      <c r="AN7" s="26"/>
-      <c r="AO7" s="26"/>
-      <c r="AP7" s="26"/>
-      <c r="AQ7" s="26"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="39"/>
+      <c r="Z7" s="39"/>
+      <c r="AA7" s="39"/>
+      <c r="AB7" s="39"/>
+      <c r="AC7" s="39"/>
+      <c r="AD7" s="39"/>
+      <c r="AE7" s="39"/>
+      <c r="AF7" s="39"/>
+      <c r="AG7" s="39"/>
+      <c r="AH7" s="39"/>
+      <c r="AI7" s="39"/>
+      <c r="AJ7" s="39"/>
+      <c r="AK7" s="39"/>
+      <c r="AL7" s="39"/>
+      <c r="AM7" s="39"/>
+      <c r="AN7" s="39"/>
+      <c r="AO7" s="39"/>
+      <c r="AP7" s="39"/>
+      <c r="AQ7" s="39"/>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
-      <c r="AD8" s="26"/>
-      <c r="AE8" s="26"/>
-      <c r="AF8" s="26"/>
-      <c r="AG8" s="26"/>
-      <c r="AH8" s="26"/>
-      <c r="AI8" s="26"/>
-      <c r="AJ8" s="26"/>
-      <c r="AK8" s="26"/>
-      <c r="AL8" s="26"/>
-      <c r="AM8" s="26"/>
-      <c r="AN8" s="26"/>
-      <c r="AO8" s="26"/>
-      <c r="AP8" s="26"/>
-      <c r="AQ8" s="26"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="39"/>
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="39"/>
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="39"/>
+      <c r="AE8" s="39"/>
+      <c r="AF8" s="39"/>
+      <c r="AG8" s="39"/>
+      <c r="AH8" s="39"/>
+      <c r="AI8" s="39"/>
+      <c r="AJ8" s="39"/>
+      <c r="AK8" s="39"/>
+      <c r="AL8" s="39"/>
+      <c r="AM8" s="39"/>
+      <c r="AN8" s="39"/>
+      <c r="AO8" s="39"/>
+      <c r="AP8" s="39"/>
+      <c r="AQ8" s="39"/>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="26"/>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
-      <c r="AH9" s="26"/>
-      <c r="AI9" s="26"/>
-      <c r="AJ9" s="26"/>
-      <c r="AK9" s="26"/>
-      <c r="AL9" s="26"/>
-      <c r="AM9" s="26"/>
-      <c r="AN9" s="26"/>
-      <c r="AO9" s="26"/>
-      <c r="AP9" s="26"/>
-      <c r="AQ9" s="26"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="39"/>
+      <c r="Z9" s="39"/>
+      <c r="AA9" s="39"/>
+      <c r="AB9" s="39"/>
+      <c r="AC9" s="39"/>
+      <c r="AD9" s="39"/>
+      <c r="AE9" s="39"/>
+      <c r="AF9" s="39"/>
+      <c r="AG9" s="39"/>
+      <c r="AH9" s="39"/>
+      <c r="AI9" s="39"/>
+      <c r="AJ9" s="39"/>
+      <c r="AK9" s="39"/>
+      <c r="AL9" s="39"/>
+      <c r="AM9" s="39"/>
+      <c r="AN9" s="39"/>
+      <c r="AO9" s="39"/>
+      <c r="AP9" s="39"/>
+      <c r="AQ9" s="39"/>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="26"/>
-      <c r="AC10" s="26"/>
-      <c r="AD10" s="26"/>
-      <c r="AE10" s="26"/>
-      <c r="AF10" s="26"/>
-      <c r="AG10" s="26"/>
-      <c r="AH10" s="26"/>
-      <c r="AI10" s="26"/>
-      <c r="AJ10" s="26"/>
-      <c r="AK10" s="26"/>
-      <c r="AL10" s="26"/>
-      <c r="AM10" s="26"/>
-      <c r="AN10" s="26"/>
-      <c r="AO10" s="26"/>
-      <c r="AP10" s="26"/>
-      <c r="AQ10" s="26"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="39"/>
+      <c r="T10" s="39"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="39"/>
+      <c r="W10" s="39"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="39"/>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="39"/>
+      <c r="AD10" s="39"/>
+      <c r="AE10" s="39"/>
+      <c r="AF10" s="39"/>
+      <c r="AG10" s="39"/>
+      <c r="AH10" s="39"/>
+      <c r="AI10" s="39"/>
+      <c r="AJ10" s="39"/>
+      <c r="AK10" s="39"/>
+      <c r="AL10" s="39"/>
+      <c r="AM10" s="39"/>
+      <c r="AN10" s="39"/>
+      <c r="AO10" s="39"/>
+      <c r="AP10" s="39"/>
+      <c r="AQ10" s="39"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="26"/>
-      <c r="AD11" s="26"/>
-      <c r="AE11" s="26"/>
-      <c r="AF11" s="26"/>
-      <c r="AG11" s="26"/>
-      <c r="AH11" s="26"/>
-      <c r="AI11" s="26"/>
-      <c r="AJ11" s="26"/>
-      <c r="AK11" s="26"/>
-      <c r="AL11" s="26"/>
-      <c r="AM11" s="26"/>
-      <c r="AN11" s="26"/>
-      <c r="AO11" s="26"/>
-      <c r="AP11" s="26"/>
-      <c r="AQ11" s="26"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="39"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="39"/>
+      <c r="Y11" s="39"/>
+      <c r="Z11" s="39"/>
+      <c r="AA11" s="39"/>
+      <c r="AB11" s="39"/>
+      <c r="AC11" s="39"/>
+      <c r="AD11" s="39"/>
+      <c r="AE11" s="39"/>
+      <c r="AF11" s="39"/>
+      <c r="AG11" s="39"/>
+      <c r="AH11" s="39"/>
+      <c r="AI11" s="39"/>
+      <c r="AJ11" s="39"/>
+      <c r="AK11" s="39"/>
+      <c r="AL11" s="39"/>
+      <c r="AM11" s="39"/>
+      <c r="AN11" s="39"/>
+      <c r="AO11" s="39"/>
+      <c r="AP11" s="39"/>
+      <c r="AQ11" s="39"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
@@ -70969,478 +70969,478 @@
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="37" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26"/>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
-      <c r="AC16" s="26"/>
-      <c r="AD16" s="26"/>
-      <c r="AE16" s="26"/>
-      <c r="AF16" s="26"/>
-      <c r="AG16" s="26"/>
-      <c r="AH16" s="26"/>
-      <c r="AI16" s="26"/>
-      <c r="AJ16" s="26"/>
-      <c r="AK16" s="26"/>
-      <c r="AL16" s="26"/>
-      <c r="AM16" s="26"/>
-      <c r="AN16" s="26"/>
-      <c r="AO16" s="26"/>
-      <c r="AP16" s="26"/>
-      <c r="AQ16" s="26"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="Z16" s="39"/>
+      <c r="AA16" s="39"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="39"/>
+      <c r="AD16" s="39"/>
+      <c r="AE16" s="39"/>
+      <c r="AF16" s="39"/>
+      <c r="AG16" s="39"/>
+      <c r="AH16" s="39"/>
+      <c r="AI16" s="39"/>
+      <c r="AJ16" s="39"/>
+      <c r="AK16" s="39"/>
+      <c r="AL16" s="39"/>
+      <c r="AM16" s="39"/>
+      <c r="AN16" s="39"/>
+      <c r="AO16" s="39"/>
+      <c r="AP16" s="39"/>
+      <c r="AQ16" s="39"/>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
-      <c r="Y17" s="26"/>
-      <c r="Z17" s="26"/>
-      <c r="AA17" s="26"/>
-      <c r="AB17" s="26"/>
-      <c r="AC17" s="26"/>
-      <c r="AD17" s="26"/>
-      <c r="AE17" s="26"/>
-      <c r="AF17" s="26"/>
-      <c r="AG17" s="26"/>
-      <c r="AH17" s="26"/>
-      <c r="AI17" s="26"/>
-      <c r="AJ17" s="26"/>
-      <c r="AK17" s="26"/>
-      <c r="AL17" s="26"/>
-      <c r="AM17" s="26"/>
-      <c r="AN17" s="26"/>
-      <c r="AO17" s="26"/>
-      <c r="AP17" s="26"/>
-      <c r="AQ17" s="26"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="39"/>
+      <c r="Y17" s="39"/>
+      <c r="Z17" s="39"/>
+      <c r="AA17" s="39"/>
+      <c r="AB17" s="39"/>
+      <c r="AC17" s="39"/>
+      <c r="AD17" s="39"/>
+      <c r="AE17" s="39"/>
+      <c r="AF17" s="39"/>
+      <c r="AG17" s="39"/>
+      <c r="AH17" s="39"/>
+      <c r="AI17" s="39"/>
+      <c r="AJ17" s="39"/>
+      <c r="AK17" s="39"/>
+      <c r="AL17" s="39"/>
+      <c r="AM17" s="39"/>
+      <c r="AN17" s="39"/>
+      <c r="AO17" s="39"/>
+      <c r="AP17" s="39"/>
+      <c r="AQ17" s="39"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="26"/>
-      <c r="AD18" s="26"/>
-      <c r="AE18" s="26"/>
-      <c r="AF18" s="26"/>
-      <c r="AG18" s="26"/>
-      <c r="AH18" s="26"/>
-      <c r="AI18" s="26"/>
-      <c r="AJ18" s="26"/>
-      <c r="AK18" s="26"/>
-      <c r="AL18" s="26"/>
-      <c r="AM18" s="26"/>
-      <c r="AN18" s="26"/>
-      <c r="AO18" s="26"/>
-      <c r="AP18" s="26"/>
-      <c r="AQ18" s="26"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="39"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="39"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="39"/>
+      <c r="W18" s="39"/>
+      <c r="X18" s="39"/>
+      <c r="Y18" s="39"/>
+      <c r="Z18" s="39"/>
+      <c r="AA18" s="39"/>
+      <c r="AB18" s="39"/>
+      <c r="AC18" s="39"/>
+      <c r="AD18" s="39"/>
+      <c r="AE18" s="39"/>
+      <c r="AF18" s="39"/>
+      <c r="AG18" s="39"/>
+      <c r="AH18" s="39"/>
+      <c r="AI18" s="39"/>
+      <c r="AJ18" s="39"/>
+      <c r="AK18" s="39"/>
+      <c r="AL18" s="39"/>
+      <c r="AM18" s="39"/>
+      <c r="AN18" s="39"/>
+      <c r="AO18" s="39"/>
+      <c r="AP18" s="39"/>
+      <c r="AQ18" s="39"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="26"/>
-      <c r="AC19" s="26"/>
-      <c r="AD19" s="26"/>
-      <c r="AE19" s="26"/>
-      <c r="AF19" s="26"/>
-      <c r="AG19" s="26"/>
-      <c r="AH19" s="26"/>
-      <c r="AI19" s="26"/>
-      <c r="AJ19" s="26"/>
-      <c r="AK19" s="26"/>
-      <c r="AL19" s="26"/>
-      <c r="AM19" s="26"/>
-      <c r="AN19" s="26"/>
-      <c r="AO19" s="26"/>
-      <c r="AP19" s="26"/>
-      <c r="AQ19" s="26"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="39"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
+      <c r="W19" s="39"/>
+      <c r="X19" s="39"/>
+      <c r="Y19" s="39"/>
+      <c r="Z19" s="39"/>
+      <c r="AA19" s="39"/>
+      <c r="AB19" s="39"/>
+      <c r="AC19" s="39"/>
+      <c r="AD19" s="39"/>
+      <c r="AE19" s="39"/>
+      <c r="AF19" s="39"/>
+      <c r="AG19" s="39"/>
+      <c r="AH19" s="39"/>
+      <c r="AI19" s="39"/>
+      <c r="AJ19" s="39"/>
+      <c r="AK19" s="39"/>
+      <c r="AL19" s="39"/>
+      <c r="AM19" s="39"/>
+      <c r="AN19" s="39"/>
+      <c r="AO19" s="39"/>
+      <c r="AP19" s="39"/>
+      <c r="AQ19" s="39"/>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-      <c r="AC20" s="26"/>
-      <c r="AD20" s="26"/>
-      <c r="AE20" s="26"/>
-      <c r="AF20" s="26"/>
-      <c r="AG20" s="26"/>
-      <c r="AH20" s="26"/>
-      <c r="AI20" s="26"/>
-      <c r="AJ20" s="26"/>
-      <c r="AK20" s="26"/>
-      <c r="AL20" s="26"/>
-      <c r="AM20" s="26"/>
-      <c r="AN20" s="26"/>
-      <c r="AO20" s="26"/>
-      <c r="AP20" s="26"/>
-      <c r="AQ20" s="26"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="39"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="39"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="39"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="39"/>
+      <c r="AD20" s="39"/>
+      <c r="AE20" s="39"/>
+      <c r="AF20" s="39"/>
+      <c r="AG20" s="39"/>
+      <c r="AH20" s="39"/>
+      <c r="AI20" s="39"/>
+      <c r="AJ20" s="39"/>
+      <c r="AK20" s="39"/>
+      <c r="AL20" s="39"/>
+      <c r="AM20" s="39"/>
+      <c r="AN20" s="39"/>
+      <c r="AO20" s="39"/>
+      <c r="AP20" s="39"/>
+      <c r="AQ20" s="39"/>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="26"/>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="26"/>
-      <c r="AC21" s="26"/>
-      <c r="AD21" s="26"/>
-      <c r="AE21" s="26"/>
-      <c r="AF21" s="26"/>
-      <c r="AG21" s="26"/>
-      <c r="AH21" s="26"/>
-      <c r="AI21" s="26"/>
-      <c r="AJ21" s="26"/>
-      <c r="AK21" s="26"/>
-      <c r="AL21" s="26"/>
-      <c r="AM21" s="26"/>
-      <c r="AN21" s="26"/>
-      <c r="AO21" s="26"/>
-      <c r="AP21" s="26"/>
-      <c r="AQ21" s="26"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="39"/>
+      <c r="Z21" s="39"/>
+      <c r="AA21" s="39"/>
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="39"/>
+      <c r="AD21" s="39"/>
+      <c r="AE21" s="39"/>
+      <c r="AF21" s="39"/>
+      <c r="AG21" s="39"/>
+      <c r="AH21" s="39"/>
+      <c r="AI21" s="39"/>
+      <c r="AJ21" s="39"/>
+      <c r="AK21" s="39"/>
+      <c r="AL21" s="39"/>
+      <c r="AM21" s="39"/>
+      <c r="AN21" s="39"/>
+      <c r="AO21" s="39"/>
+      <c r="AP21" s="39"/>
+      <c r="AQ21" s="39"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="26"/>
-      <c r="AD22" s="26"/>
-      <c r="AE22" s="26"/>
-      <c r="AF22" s="26"/>
-      <c r="AG22" s="26"/>
-      <c r="AH22" s="26"/>
-      <c r="AI22" s="26"/>
-      <c r="AJ22" s="26"/>
-      <c r="AK22" s="26"/>
-      <c r="AL22" s="26"/>
-      <c r="AM22" s="26"/>
-      <c r="AN22" s="26"/>
-      <c r="AO22" s="26"/>
-      <c r="AP22" s="26"/>
-      <c r="AQ22" s="26"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="39"/>
+      <c r="S22" s="39"/>
+      <c r="T22" s="39"/>
+      <c r="U22" s="39"/>
+      <c r="V22" s="39"/>
+      <c r="W22" s="39"/>
+      <c r="X22" s="39"/>
+      <c r="Y22" s="39"/>
+      <c r="Z22" s="39"/>
+      <c r="AA22" s="39"/>
+      <c r="AB22" s="39"/>
+      <c r="AC22" s="39"/>
+      <c r="AD22" s="39"/>
+      <c r="AE22" s="39"/>
+      <c r="AF22" s="39"/>
+      <c r="AG22" s="39"/>
+      <c r="AH22" s="39"/>
+      <c r="AI22" s="39"/>
+      <c r="AJ22" s="39"/>
+      <c r="AK22" s="39"/>
+      <c r="AL22" s="39"/>
+      <c r="AM22" s="39"/>
+      <c r="AN22" s="39"/>
+      <c r="AO22" s="39"/>
+      <c r="AP22" s="39"/>
+      <c r="AQ22" s="39"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="26"/>
-      <c r="AC23" s="26"/>
-      <c r="AD23" s="26"/>
-      <c r="AE23" s="26"/>
-      <c r="AF23" s="26"/>
-      <c r="AG23" s="26"/>
-      <c r="AH23" s="26"/>
-      <c r="AI23" s="26"/>
-      <c r="AJ23" s="26"/>
-      <c r="AK23" s="26"/>
-      <c r="AL23" s="26"/>
-      <c r="AM23" s="26"/>
-      <c r="AN23" s="26"/>
-      <c r="AO23" s="26"/>
-      <c r="AP23" s="26"/>
-      <c r="AQ23" s="26"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="39"/>
+      <c r="X23" s="39"/>
+      <c r="Y23" s="39"/>
+      <c r="Z23" s="39"/>
+      <c r="AA23" s="39"/>
+      <c r="AB23" s="39"/>
+      <c r="AC23" s="39"/>
+      <c r="AD23" s="39"/>
+      <c r="AE23" s="39"/>
+      <c r="AF23" s="39"/>
+      <c r="AG23" s="39"/>
+      <c r="AH23" s="39"/>
+      <c r="AI23" s="39"/>
+      <c r="AJ23" s="39"/>
+      <c r="AK23" s="39"/>
+      <c r="AL23" s="39"/>
+      <c r="AM23" s="39"/>
+      <c r="AN23" s="39"/>
+      <c r="AO23" s="39"/>
+      <c r="AP23" s="39"/>
+      <c r="AQ23" s="39"/>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-      <c r="AC24" s="26"/>
-      <c r="AD24" s="26"/>
-      <c r="AE24" s="26"/>
-      <c r="AF24" s="26"/>
-      <c r="AG24" s="26"/>
-      <c r="AH24" s="26"/>
-      <c r="AI24" s="26"/>
-      <c r="AJ24" s="26"/>
-      <c r="AK24" s="26"/>
-      <c r="AL24" s="26"/>
-      <c r="AM24" s="26"/>
-      <c r="AN24" s="26"/>
-      <c r="AO24" s="26"/>
-      <c r="AP24" s="26"/>
-      <c r="AQ24" s="26"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="39"/>
+      <c r="S24" s="39"/>
+      <c r="T24" s="39"/>
+      <c r="U24" s="39"/>
+      <c r="V24" s="39"/>
+      <c r="W24" s="39"/>
+      <c r="X24" s="39"/>
+      <c r="Y24" s="39"/>
+      <c r="Z24" s="39"/>
+      <c r="AA24" s="39"/>
+      <c r="AB24" s="39"/>
+      <c r="AC24" s="39"/>
+      <c r="AD24" s="39"/>
+      <c r="AE24" s="39"/>
+      <c r="AF24" s="39"/>
+      <c r="AG24" s="39"/>
+      <c r="AH24" s="39"/>
+      <c r="AI24" s="39"/>
+      <c r="AJ24" s="39"/>
+      <c r="AK24" s="39"/>
+      <c r="AL24" s="39"/>
+      <c r="AM24" s="39"/>
+      <c r="AN24" s="39"/>
+      <c r="AO24" s="39"/>
+      <c r="AP24" s="39"/>
+      <c r="AQ24" s="39"/>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="26"/>
-      <c r="AC25" s="26"/>
-      <c r="AD25" s="26"/>
-      <c r="AE25" s="26"/>
-      <c r="AF25" s="26"/>
-      <c r="AG25" s="26"/>
-      <c r="AH25" s="26"/>
-      <c r="AI25" s="26"/>
-      <c r="AJ25" s="26"/>
-      <c r="AK25" s="26"/>
-      <c r="AL25" s="26"/>
-      <c r="AM25" s="26"/>
-      <c r="AN25" s="26"/>
-      <c r="AO25" s="26"/>
-      <c r="AP25" s="26"/>
-      <c r="AQ25" s="26"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="39"/>
+      <c r="T25" s="39"/>
+      <c r="U25" s="39"/>
+      <c r="V25" s="39"/>
+      <c r="W25" s="39"/>
+      <c r="X25" s="39"/>
+      <c r="Y25" s="39"/>
+      <c r="Z25" s="39"/>
+      <c r="AA25" s="39"/>
+      <c r="AB25" s="39"/>
+      <c r="AC25" s="39"/>
+      <c r="AD25" s="39"/>
+      <c r="AE25" s="39"/>
+      <c r="AF25" s="39"/>
+      <c r="AG25" s="39"/>
+      <c r="AH25" s="39"/>
+      <c r="AI25" s="39"/>
+      <c r="AJ25" s="39"/>
+      <c r="AK25" s="39"/>
+      <c r="AL25" s="39"/>
+      <c r="AM25" s="39"/>
+      <c r="AN25" s="39"/>
+      <c r="AO25" s="39"/>
+      <c r="AP25" s="39"/>
+      <c r="AQ25" s="39"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
@@ -71934,7 +71934,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -71974,8 +71974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -71987,485 +71987,485 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="29"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="A1" s="24"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+        <v>84</v>
+      </c>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>121</v>
+      <c r="A2" s="25"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>125</v>
+      <c r="A3" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="36">
+      <c r="A4" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="30">
         <v>1</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="33">
         <v>2018</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="34">
         <v>1</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="27">
         <v>0</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="27">
         <v>0</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="37">
+      <c r="A5" s="25"/>
+      <c r="B5" s="31">
         <v>2</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="42">
+      <c r="C5" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="35">
         <v>1</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="28">
         <v>0</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="28">
         <v>0</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="37">
+      <c r="A6" s="25"/>
+      <c r="B6" s="31">
         <v>3</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="42">
+      <c r="C6" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="35">
         <v>0.97570000000000001</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="28">
         <v>2.4299999999999999E-2</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="28">
         <v>0</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="37">
+      <c r="A7" s="25"/>
+      <c r="B7" s="31">
         <v>4</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="42">
+      <c r="C7" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="35">
         <v>0.89580000000000004</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="28">
         <v>0.1042</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="28">
         <v>0</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
-      <c r="B8" s="38">
+      <c r="A8" s="26"/>
+      <c r="B8" s="32">
         <v>5</v>
       </c>
-      <c r="C8" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" s="43">
+      <c r="C8" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="36">
         <v>0.93400000000000005</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="29">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="29">
         <v>0</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="36">
+      <c r="A9" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="30">
         <v>1</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="33">
         <v>2018</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="34">
         <v>1</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="27">
         <v>0</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="27">
         <v>0</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="37">
+      <c r="A10" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="31">
         <v>2</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="42">
+      <c r="C10" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="35">
         <v>0.54859999999999998</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="28">
         <v>0.22220000000000001</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="28">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="28">
         <v>0.1875</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="37">
+      <c r="A11" s="25"/>
+      <c r="B11" s="31">
         <v>3</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="42">
+      <c r="C11" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="35">
         <v>0.31769999999999998</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="28">
         <v>1.5599999999999999E-2</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="28">
         <v>0.1042</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="28">
         <v>0.5625</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
-      <c r="B12" s="37">
+      <c r="A12" s="25"/>
+      <c r="B12" s="31">
         <v>4</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="42">
+      <c r="C12" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="35">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="28">
         <v>0.12670000000000001</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="28">
         <v>0.17710000000000001</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="28">
         <v>0.64059999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="38">
+      <c r="A13" s="26"/>
+      <c r="B13" s="32">
         <v>5</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="43">
+      <c r="C13" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="36">
         <v>0</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="29">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="29">
         <v>3.6499999999999998E-2</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="29">
         <v>0.96179999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" s="36">
+      <c r="A14" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="30">
         <v>1</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="33">
         <v>2018</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="34">
         <v>1</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="27">
         <v>0</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="27">
         <v>0</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
-      <c r="B15" s="37">
+      <c r="A15" s="25"/>
+      <c r="B15" s="31">
         <v>2</v>
       </c>
-      <c r="C15" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="42">
+      <c r="C15" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="35">
         <v>0.59379999999999999</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="28">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="28">
         <v>0.15629999999999999</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="28">
         <v>0.1719</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
-      <c r="B16" s="37">
+      <c r="A16" s="25"/>
+      <c r="B16" s="31">
         <v>3</v>
       </c>
-      <c r="C16" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" s="42">
+      <c r="C16" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="35">
         <v>0.65100000000000002</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="28">
         <v>9.3799999999999994E-2</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F16" s="28">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="28">
         <v>0.1719</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
-      <c r="B17" s="37">
+      <c r="A17" s="25"/>
+      <c r="B17" s="31">
         <v>4</v>
       </c>
-      <c r="C17" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="42">
+      <c r="C17" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="35">
         <v>0.4531</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="28">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="28">
         <v>5.7299999999999997E-2</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="28">
         <v>0.44790000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
-      <c r="B18" s="38">
+      <c r="A18" s="26"/>
+      <c r="B18" s="32">
         <v>5</v>
       </c>
-      <c r="C18" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="43">
+      <c r="C18" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="36">
         <v>0.62760000000000005</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="29">
         <v>5.9900000000000002E-2</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="29">
         <v>2.3400000000000001E-2</v>
       </c>
-      <c r="G18" s="35">
+      <c r="G18" s="29">
         <v>0.28910000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" s="36">
+      <c r="A19" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="30">
         <v>1</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="33">
         <v>2018</v>
       </c>
-      <c r="D19" s="41">
+      <c r="D19" s="34">
         <v>1</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="27">
         <v>0</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="27">
         <v>0</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B20" s="37">
+      <c r="A20" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="31">
         <v>2</v>
       </c>
-      <c r="C20" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="42">
+      <c r="C20" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="35">
         <v>0.24540000000000001</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="28">
         <v>0.12959999999999999</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="28">
         <v>3.9399999999999998E-2</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="28">
         <v>0.58560000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
-      <c r="B21" s="37">
+      <c r="A21" s="25"/>
+      <c r="B21" s="31">
         <v>3</v>
       </c>
-      <c r="C21" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="42">
+      <c r="C21" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="35">
         <v>9.7199999999999995E-2</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="28">
         <v>4.6300000000000001E-2</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="28">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="28">
         <v>0.83450000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="37">
+      <c r="A22" s="25"/>
+      <c r="B22" s="31">
         <v>4</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" s="42">
+      <c r="C22" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="35">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="28">
         <v>8.0999999999999996E-3</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="28">
         <v>2.4299999999999999E-2</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="28">
         <v>0.96060000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="32"/>
-      <c r="B23" s="38">
+      <c r="A23" s="26"/>
+      <c r="B23" s="32">
         <v>5</v>
       </c>
-      <c r="C23" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="43">
+      <c r="C23" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="36">
         <v>0</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="29">
         <v>0</v>
       </c>
-      <c r="F23" s="35">
+      <c r="F23" s="29">
         <v>0</v>
       </c>
-      <c r="G23" s="35">
+      <c r="G23" s="29">
         <v>1</v>
       </c>
     </row>
@@ -72504,56 +72504,56 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="N1" s="28" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="N1" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="N2" s="27" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="N2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -74932,56 +74932,56 @@
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="N40" s="28" t="s">
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+      <c r="N40" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="O40" s="28"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="28"/>
-      <c r="W40" s="28"/>
+      <c r="O40" s="43"/>
+      <c r="P40" s="43"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="43"/>
+      <c r="T40" s="43"/>
+      <c r="U40" s="43"/>
+      <c r="V40" s="43"/>
+      <c r="W40" s="43"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="N41" s="27" t="s">
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="42"/>
+      <c r="N41" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="27"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="42"/>
+      <c r="Q41" s="42"/>
+      <c r="R41" s="42"/>
+      <c r="S41" s="42"/>
+      <c r="T41" s="42"/>
+      <c r="U41" s="42"/>
+      <c r="V41" s="42"/>
+      <c r="W41" s="42"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" t="s">

</xml_diff>